<commit_message>
chore: remove redundant fields
</commit_message>
<xml_diff>
--- a/src/assets/signs.xlsx
+++ b/src/assets/signs.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="859" uniqueCount="738">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="731">
   <si>
     <t>1.1</t>
   </si>
@@ -1450,15 +1450,6 @@
     <t>Маршрут движения на перекрестке в случае запрещения отдельных манёвров, указание разрешённых направлений движения на перекрестке со сложной планировкой.</t>
   </si>
   <si>
-    <t>5.20.4</t>
-  </si>
-  <si>
-    <t>Схема движения к пункту обслуживания системы электронного сбора платы за проезд</t>
-  </si>
-  <si>
-    <t>Указывает направление движения к пункту обслуживания системы BelToll. Рекомендательный[9].</t>
-  </si>
-  <si>
     <t>5.21.1</t>
   </si>
   <si>
@@ -1558,12 +1549,6 @@
     <t>Номер дороги, на которой установлен данный знак.На знаках 5.29.1, 5.29.3 с зелёным фоном указывается номер дороги, включенной в Европейскую систему автомобильных магистралей, с красным фоном — номер магистральной или республиканской дороги, с белым фоном — номер местной дороги.</t>
   </si>
   <si>
-    <t>5.29.2</t>
-  </si>
-  <si>
-    <t>Номер дороги, в направлении к которой осуществляется движение.</t>
-  </si>
-  <si>
     <t>5.29.3</t>
   </si>
   <si>
@@ -1709,12 +1694,6 @@
   </si>
   <si>
     <t>Знак информирует о конце участка дороги, на котором используется система электронного сбора платы в режиме свободного многополосного движения за проезд транспортных средств.</t>
-  </si>
-  <si>
-    <t>5.44</t>
-  </si>
-  <si>
-    <t>Указатель направления к пункту обслуживания системы электронного сбора платы за проезд</t>
   </si>
   <si>
     <t>6.1</t>
@@ -2235,10 +2214,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-* #\.##0\ &quot;₽&quot;_-;\-* #\.##0\ &quot;₽&quot;_-;_-* \-\ &quot;₽&quot;_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-* #\.##0.00\ &quot;₽&quot;_-;\-* #\.##0.00\ &quot;₽&quot;_-;_-* \-??\ &quot;₽&quot;_-;_-@_-"/>
     <numFmt numFmtId="177" formatCode="_-* #\.##0.00_-;\-* #\.##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-* #\.##0_-;\-* #\.##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-* #\.##0.00\ &quot;₽&quot;_-;\-* #\.##0.00\ &quot;₽&quot;_-;_-* \-??\ &quot;₽&quot;_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-* #\.##0\ &quot;₽&quot;_-;\-* #\.##0\ &quot;₽&quot;_-;_-* \-\ &quot;₽&quot;_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-* #\.##0_-;\-* #\.##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -2261,16 +2240,8 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2283,6 +2254,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -2290,25 +2269,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2330,6 +2307,37 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -2337,17 +2345,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2369,39 +2376,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -2414,7 +2393,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2426,7 +2417,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2438,19 +2525,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2462,139 +2561,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2608,25 +2587,40 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
+      <right style="double">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
+      <top style="double">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
+      <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -2644,16 +2638,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2685,171 +2679,156 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -3205,10 +3184,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E302"/>
+  <dimension ref="A1:E299"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A292" workbookViewId="0">
-      <selection activeCell="E303" sqref="E303"/>
+      <selection activeCell="B302" sqref="B302"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.75" outlineLevelCol="4"/>
@@ -3725,7 +3704,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="29" ht="15.75" spans="1:5">
+    <row r="29" spans="1:5">
       <c r="A29" s="7">
         <v>29</v>
       </c>
@@ -3743,7 +3722,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="30" ht="15.75" spans="1:5">
+    <row r="30" spans="1:5">
       <c r="A30" s="7">
         <v>30</v>
       </c>
@@ -3759,7 +3738,7 @@
       </c>
       <c r="E30" s="11"/>
     </row>
-    <row r="31" ht="15.75" spans="1:5">
+    <row r="31" spans="1:5">
       <c r="A31" s="7">
         <v>31</v>
       </c>
@@ -3775,7 +3754,7 @@
       </c>
       <c r="E31" s="11"/>
     </row>
-    <row r="32" ht="15.75" spans="1:5">
+    <row r="32" spans="1:5">
       <c r="A32" s="7">
         <v>32</v>
       </c>
@@ -3791,7 +3770,7 @@
       </c>
       <c r="E32" s="11"/>
     </row>
-    <row r="33" ht="15.75" spans="1:5">
+    <row r="33" spans="1:5">
       <c r="A33" s="7">
         <v>33</v>
       </c>
@@ -3807,7 +3786,7 @@
       </c>
       <c r="E33" s="11"/>
     </row>
-    <row r="34" ht="15.75" spans="1:5">
+    <row r="34" spans="1:5">
       <c r="A34" s="7">
         <v>34</v>
       </c>
@@ -4075,7 +4054,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="49" ht="15.75" spans="1:5">
+    <row r="49" spans="1:5">
       <c r="A49" s="7">
         <v>49</v>
       </c>
@@ -4091,7 +4070,7 @@
       </c>
       <c r="E49" s="11"/>
     </row>
-    <row r="50" ht="15.75" spans="1:5">
+    <row r="50" spans="1:5">
       <c r="A50" s="7">
         <v>50</v>
       </c>
@@ -4107,7 +4086,7 @@
       </c>
       <c r="E50" s="11"/>
     </row>
-    <row r="51" ht="15.75" spans="1:5">
+    <row r="51" spans="1:5">
       <c r="A51" s="7">
         <v>51</v>
       </c>
@@ -4123,7 +4102,7 @@
       </c>
       <c r="E51" s="11"/>
     </row>
-    <row r="52" ht="15.75" spans="1:5">
+    <row r="52" spans="1:5">
       <c r="A52" s="7">
         <v>52</v>
       </c>
@@ -4445,7 +4424,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="70" ht="15.75" spans="1:5">
+    <row r="70" spans="1:5">
       <c r="A70" s="7">
         <v>70</v>
       </c>
@@ -4463,7 +4442,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="71" ht="15.75" spans="1:5">
+    <row r="71" spans="1:5">
       <c r="A71" s="7">
         <v>71</v>
       </c>
@@ -4499,7 +4478,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="73" ht="15.75" spans="1:5">
+    <row r="73" spans="1:5">
       <c r="A73" s="7">
         <v>73</v>
       </c>
@@ -4517,7 +4496,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="74" ht="15.75" spans="1:5">
+    <row r="74" spans="1:5">
       <c r="A74" s="7">
         <v>74</v>
       </c>
@@ -4571,7 +4550,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="77" ht="15.75" spans="1:5">
+    <row r="77" spans="1:5">
       <c r="A77" s="7">
         <v>77</v>
       </c>
@@ -4589,7 +4568,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="78" ht="15.75" spans="1:5">
+    <row r="78" spans="1:5">
       <c r="A78" s="7">
         <v>78</v>
       </c>
@@ -4805,7 +4784,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="90" ht="15.75" spans="1:5">
+    <row r="90" spans="1:5">
       <c r="A90" s="7">
         <v>90</v>
       </c>
@@ -4823,7 +4802,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="91" ht="15.75" spans="1:5">
+    <row r="91" spans="1:5">
       <c r="A91" s="7">
         <v>91</v>
       </c>
@@ -4841,7 +4820,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="92" ht="15.75" spans="1:5">
+    <row r="92" spans="1:5">
       <c r="A92" s="7">
         <v>92</v>
       </c>
@@ -4877,7 +4856,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="94" ht="15.75" spans="1:5">
+    <row r="94" spans="1:5">
       <c r="A94" s="7">
         <v>94</v>
       </c>
@@ -4911,7 +4890,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="96" ht="15.75" spans="1:5">
+    <row r="96" spans="1:5">
       <c r="A96" s="7">
         <v>96</v>
       </c>
@@ -4929,7 +4908,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="97" ht="15.75" spans="1:5">
+    <row r="97" spans="1:5">
       <c r="A97" s="7">
         <v>97</v>
       </c>
@@ -4965,7 +4944,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="99" ht="15.75" spans="1:5">
+    <row r="99" spans="1:5">
       <c r="A99" s="7">
         <v>99</v>
       </c>
@@ -5019,7 +4998,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="102" ht="15.75" spans="1:5">
+    <row r="102" spans="1:5">
       <c r="A102" s="7">
         <v>102</v>
       </c>
@@ -5037,7 +5016,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="103" ht="15.75" spans="1:5">
+    <row r="103" spans="1:5">
       <c r="A103" s="7">
         <v>103</v>
       </c>
@@ -5071,7 +5050,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="105" ht="15.75" spans="1:5">
+    <row r="105" spans="1:5">
       <c r="A105" s="7">
         <v>105</v>
       </c>
@@ -5089,7 +5068,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="106" ht="15.75" spans="1:5">
+    <row r="106" spans="1:5">
       <c r="A106" s="7">
         <v>106</v>
       </c>
@@ -5107,7 +5086,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="107" ht="15.75" spans="1:5">
+    <row r="107" spans="1:5">
       <c r="A107" s="7">
         <v>107</v>
       </c>
@@ -5179,7 +5158,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="111" ht="15.75" spans="1:5">
+    <row r="111" spans="1:5">
       <c r="A111" s="7">
         <v>111</v>
       </c>
@@ -5197,7 +5176,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="112" ht="15.75" spans="1:5">
+    <row r="112" spans="1:5">
       <c r="A112" s="7">
         <v>112</v>
       </c>
@@ -5233,7 +5212,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="114" ht="15.75" spans="1:5">
+    <row r="114" spans="1:5">
       <c r="A114" s="7">
         <v>114</v>
       </c>
@@ -5359,7 +5338,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="121" ht="15.75" spans="1:5">
+    <row r="121" spans="1:5">
       <c r="A121" s="7">
         <v>121</v>
       </c>
@@ -5395,7 +5374,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="123" ht="15.75" spans="1:5">
+    <row r="123" spans="1:5">
       <c r="A123" s="7">
         <v>123</v>
       </c>
@@ -5467,7 +5446,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="127" ht="15.75" spans="1:5">
+    <row r="127" spans="1:5">
       <c r="A127" s="7">
         <v>127</v>
       </c>
@@ -5539,7 +5518,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="131" ht="15.75" spans="1:5">
+    <row r="131" spans="1:5">
       <c r="A131" s="7">
         <v>131</v>
       </c>
@@ -5611,7 +5590,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="135" ht="15.75" spans="1:5">
+    <row r="135" spans="1:5">
       <c r="A135" s="7">
         <v>135</v>
       </c>
@@ -5629,7 +5608,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="136" ht="15.75" spans="1:5">
+    <row r="136" spans="1:5">
       <c r="A136" s="7">
         <v>136</v>
       </c>
@@ -5683,7 +5662,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="139" ht="15.75" spans="1:5">
+    <row r="139" spans="1:5">
       <c r="A139" s="7">
         <v>139</v>
       </c>
@@ -5701,7 +5680,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="140" ht="15.75" spans="1:5">
+    <row r="140" spans="1:5">
       <c r="A140" s="7">
         <v>140</v>
       </c>
@@ -5773,7 +5752,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="144" ht="15.75" spans="1:5">
+    <row r="144" spans="1:5">
       <c r="A144" s="7">
         <v>144</v>
       </c>
@@ -5809,7 +5788,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="146" ht="15.75" spans="1:5">
+    <row r="146" spans="1:5">
       <c r="A146" s="7">
         <v>146</v>
       </c>
@@ -5935,7 +5914,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="153" ht="15.75" spans="1:5">
+    <row r="153" spans="1:5">
       <c r="A153" s="7">
         <v>153</v>
       </c>
@@ -5953,7 +5932,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="154" ht="15.75" spans="1:5">
+    <row r="154" spans="1:5">
       <c r="A154" s="7">
         <v>154</v>
       </c>
@@ -5989,7 +5968,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="156" ht="15.75" spans="1:5">
+    <row r="156" spans="1:5">
       <c r="A156" s="7">
         <v>156</v>
       </c>
@@ -6023,7 +6002,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="158" ht="15.75" spans="1:5">
+    <row r="158" spans="1:5">
       <c r="A158" s="7">
         <v>158</v>
       </c>
@@ -6095,7 +6074,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="162" ht="15.75" spans="1:5">
+    <row r="162" spans="1:5">
       <c r="A162" s="7">
         <v>162</v>
       </c>
@@ -6131,7 +6110,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="164" ht="15.75" spans="1:5">
+    <row r="164" spans="1:5">
       <c r="A164" s="7">
         <v>164</v>
       </c>
@@ -6226,7 +6205,7 @@
         <v>169</v>
       </c>
       <c r="B169" s="8" t="str">
-        <f t="shared" ref="B169:B232" si="4">C169&amp;".svg"</f>
+        <f t="shared" ref="B169:B196" si="4">C169&amp;".svg"</f>
         <v>5.14.1.svg</v>
       </c>
       <c r="C169" s="9" t="s">
@@ -6293,7 +6272,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="173" ht="15.75" spans="1:5">
+    <row r="173" spans="1:5">
       <c r="A173" s="7">
         <v>173</v>
       </c>
@@ -6325,7 +6304,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="175" ht="15.75" spans="1:5">
+    <row r="175" spans="1:5">
       <c r="A175" s="7">
         <v>175</v>
       </c>
@@ -6357,7 +6336,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="177" ht="15.75" spans="1:5">
+    <row r="177" spans="1:5">
       <c r="A177" s="7">
         <v>177</v>
       </c>
@@ -6389,7 +6368,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="179" ht="15.75" spans="1:5">
+    <row r="179" spans="1:5">
       <c r="A179" s="7">
         <v>179</v>
       </c>
@@ -6479,13 +6458,13 @@
         <v>477</v>
       </c>
     </row>
-    <row r="184" ht="31.5" spans="1:5">
+    <row r="184" ht="78.75" spans="1:5">
       <c r="A184" s="7">
         <v>184</v>
       </c>
       <c r="B184" s="8" t="str">
         <f t="shared" si="4"/>
-        <v>5.20.4.svg</v>
+        <v>5.21.1.svg</v>
       </c>
       <c r="C184" s="9" t="s">
         <v>478</v>
@@ -6497,13 +6476,13 @@
         <v>480</v>
       </c>
     </row>
-    <row r="185" ht="78.75" spans="1:5">
+    <row r="185" spans="1:5">
       <c r="A185" s="7">
         <v>185</v>
       </c>
       <c r="B185" s="8" t="str">
         <f t="shared" si="4"/>
-        <v>5.21.1.svg</v>
+        <v>5.21.2.svg</v>
       </c>
       <c r="C185" s="9" t="s">
         <v>481</v>
@@ -6511,101 +6490,101 @@
       <c r="D185" s="10" t="s">
         <v>482</v>
       </c>
-      <c r="E185" s="11" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="186" ht="15.75" spans="1:5">
+      <c r="E185" s="11"/>
+    </row>
+    <row r="186" ht="47.25" spans="1:5">
       <c r="A186" s="7">
         <v>186</v>
       </c>
       <c r="B186" s="8" t="str">
         <f t="shared" si="4"/>
-        <v>5.21.2.svg</v>
+        <v>5.22.1.svg</v>
       </c>
       <c r="C186" s="9" t="s">
+        <v>483</v>
+      </c>
+      <c r="D186" s="10" t="s">
         <v>484</v>
       </c>
-      <c r="D186" s="10" t="s">
+      <c r="E186" s="11" t="s">
         <v>485</v>
       </c>
-      <c r="E186" s="11"/>
-    </row>
-    <row r="187" ht="47.25" spans="1:5">
+    </row>
+    <row r="187" spans="1:5">
       <c r="A187" s="7">
         <v>187</v>
       </c>
       <c r="B187" s="8" t="str">
         <f t="shared" si="4"/>
-        <v>5.22.1.svg</v>
+        <v>5.22.2.svg</v>
       </c>
       <c r="C187" s="9" t="s">
         <v>486</v>
       </c>
       <c r="D187" s="10" t="s">
-        <v>487</v>
-      </c>
-      <c r="E187" s="11" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="188" ht="15.75" spans="1:5">
+        <v>484</v>
+      </c>
+      <c r="E187" s="11"/>
+    </row>
+    <row r="188" ht="31.5" spans="1:5">
       <c r="A188" s="7">
         <v>188</v>
       </c>
       <c r="B188" s="8" t="str">
         <f t="shared" si="4"/>
-        <v>5.22.2.svg</v>
+        <v>5.23.1.svg</v>
       </c>
       <c r="C188" s="9" t="s">
+        <v>487</v>
+      </c>
+      <c r="D188" s="10" t="s">
+        <v>488</v>
+      </c>
+      <c r="E188" s="11" t="s">
         <v>489</v>
       </c>
-      <c r="D188" s="10" t="s">
-        <v>487</v>
-      </c>
-      <c r="E188" s="11"/>
-    </row>
-    <row r="189" ht="31.5" spans="1:5">
+    </row>
+    <row r="189" spans="1:5">
       <c r="A189" s="7">
         <v>189</v>
       </c>
       <c r="B189" s="8" t="str">
         <f t="shared" si="4"/>
-        <v>5.23.1.svg</v>
+        <v>5.23.2.svg</v>
       </c>
       <c r="C189" s="9" t="s">
         <v>490</v>
       </c>
       <c r="D189" s="10" t="s">
-        <v>491</v>
-      </c>
-      <c r="E189" s="11" t="s">
-        <v>492</v>
-      </c>
-    </row>
-    <row r="190" ht="15.75" spans="1:5">
+        <v>488</v>
+      </c>
+      <c r="E189" s="11"/>
+    </row>
+    <row r="190" ht="47.25" spans="1:5">
       <c r="A190" s="7">
         <v>190</v>
       </c>
       <c r="B190" s="8" t="str">
         <f t="shared" si="4"/>
-        <v>5.23.2.svg</v>
+        <v>5.24.svg</v>
       </c>
       <c r="C190" s="9" t="s">
+        <v>491</v>
+      </c>
+      <c r="D190" s="10" t="s">
+        <v>492</v>
+      </c>
+      <c r="E190" s="11" t="s">
         <v>493</v>
       </c>
-      <c r="D190" s="10" t="s">
-        <v>491</v>
-      </c>
-      <c r="E190" s="11"/>
-    </row>
-    <row r="191" ht="47.25" spans="1:5">
+    </row>
+    <row r="191" spans="1:5">
       <c r="A191" s="7">
         <v>191</v>
       </c>
       <c r="B191" s="8" t="str">
         <f t="shared" si="4"/>
-        <v>5.24.svg</v>
+        <v>5.25.svg</v>
       </c>
       <c r="C191" s="9" t="s">
         <v>494</v>
@@ -6617,13 +6596,13 @@
         <v>496</v>
       </c>
     </row>
-    <row r="192" ht="15.75" spans="1:5">
+    <row r="192" ht="47.25" spans="1:5">
       <c r="A192" s="7">
         <v>192</v>
       </c>
       <c r="B192" s="8" t="str">
         <f t="shared" si="4"/>
-        <v>5.25.svg</v>
+        <v>5.26.1.svg</v>
       </c>
       <c r="C192" s="9" t="s">
         <v>497</v>
@@ -6635,49 +6614,49 @@
         <v>499</v>
       </c>
     </row>
-    <row r="193" ht="47.25" spans="1:5">
+    <row r="193" ht="31.5" spans="1:5">
       <c r="A193" s="7">
         <v>193</v>
       </c>
       <c r="B193" s="8" t="str">
         <f t="shared" si="4"/>
-        <v>5.26.1.svg</v>
+        <v>5.26.2.svg</v>
       </c>
       <c r="C193" s="9" t="s">
         <v>500</v>
       </c>
       <c r="D193" s="10" t="s">
+        <v>498</v>
+      </c>
+      <c r="E193" s="10" t="s">
         <v>501</v>
       </c>
-      <c r="E193" s="11" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="194" ht="31.5" spans="1:5">
+    </row>
+    <row r="194" spans="1:5">
       <c r="A194" s="7">
         <v>194</v>
       </c>
       <c r="B194" s="8" t="str">
         <f t="shared" si="4"/>
-        <v>5.26.2.svg</v>
+        <v>5.27.svg</v>
       </c>
       <c r="C194" s="9" t="s">
+        <v>502</v>
+      </c>
+      <c r="D194" s="10" t="s">
         <v>503</v>
       </c>
-      <c r="D194" s="10" t="s">
-        <v>501</v>
-      </c>
-      <c r="E194" s="10" t="s">
+      <c r="E194" s="11" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="195" ht="15.75" spans="1:5">
+    <row r="195" spans="1:5">
       <c r="A195" s="7">
         <v>195</v>
       </c>
       <c r="B195" s="8" t="str">
         <f t="shared" si="4"/>
-        <v>5.27.svg</v>
+        <v>5.28.svg</v>
       </c>
       <c r="C195" s="9" t="s">
         <v>505</v>
@@ -6689,13 +6668,13 @@
         <v>507</v>
       </c>
     </row>
-    <row r="196" ht="15.75" spans="1:5">
+    <row r="196" ht="78.75" spans="1:5">
       <c r="A196" s="7">
         <v>196</v>
       </c>
       <c r="B196" s="8" t="str">
         <f t="shared" si="4"/>
-        <v>5.28.svg</v>
+        <v>5.29.1.svg</v>
       </c>
       <c r="C196" s="9" t="s">
         <v>508</v>
@@ -6707,13 +6686,13 @@
         <v>510</v>
       </c>
     </row>
-    <row r="197" ht="78.75" spans="1:5">
+    <row r="197" ht="31.5" spans="1:5">
       <c r="A197" s="7">
         <v>197</v>
       </c>
       <c r="B197" s="8" t="str">
-        <f t="shared" si="4"/>
-        <v>5.29.1.svg</v>
+        <f t="shared" ref="B197:B230" si="5">C197&amp;".svg"</f>
+        <v>5.29.3.svg</v>
       </c>
       <c r="C197" s="9" t="s">
         <v>511</v>
@@ -6725,40 +6704,40 @@
         <v>513</v>
       </c>
     </row>
-    <row r="198" ht="15.75" spans="1:5">
+    <row r="198" ht="47.25" spans="1:5">
       <c r="A198" s="7">
         <v>198</v>
       </c>
       <c r="B198" s="8" t="str">
-        <f t="shared" si="4"/>
-        <v>5.29.2.svg</v>
+        <f t="shared" si="5"/>
+        <v>5.30.1.svg</v>
       </c>
       <c r="C198" s="9" t="s">
         <v>514</v>
       </c>
       <c r="D198" s="10" t="s">
-        <v>512</v>
-      </c>
-      <c r="E198" s="10" t="s">
         <v>515</v>
       </c>
-    </row>
-    <row r="199" ht="31.5" spans="1:5">
+      <c r="E198" s="11" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="199" ht="47.25" spans="1:5">
       <c r="A199" s="7">
         <v>199</v>
       </c>
       <c r="B199" s="8" t="str">
-        <f t="shared" si="4"/>
-        <v>5.29.3.svg</v>
+        <f t="shared" si="5"/>
+        <v>5.30.2.svg</v>
       </c>
       <c r="C199" s="9" t="s">
+        <v>517</v>
+      </c>
+      <c r="D199" s="10" t="s">
+        <v>515</v>
+      </c>
+      <c r="E199" s="11" t="s">
         <v>516</v>
-      </c>
-      <c r="D199" s="10" t="s">
-        <v>517</v>
-      </c>
-      <c r="E199" s="11" t="s">
-        <v>518</v>
       </c>
     </row>
     <row r="200" ht="47.25" spans="1:5">
@@ -6766,29 +6745,29 @@
         <v>200</v>
       </c>
       <c r="B200" s="8" t="str">
-        <f t="shared" si="4"/>
-        <v>5.30.1.svg</v>
+        <f t="shared" si="5"/>
+        <v>5.30.3.svg</v>
       </c>
       <c r="C200" s="9" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D200" s="10" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
       <c r="E200" s="11" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="201" ht="47.25" spans="1:5">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5">
       <c r="A201" s="7">
         <v>201</v>
       </c>
       <c r="B201" s="8" t="str">
-        <f t="shared" si="4"/>
-        <v>5.30.2.svg</v>
+        <f t="shared" si="5"/>
+        <v>5.31.svg</v>
       </c>
       <c r="C201" s="9" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="D201" s="10" t="s">
         <v>520</v>
@@ -6797,70 +6776,70 @@
         <v>521</v>
       </c>
     </row>
-    <row r="202" ht="47.25" spans="1:5">
+    <row r="202" spans="1:5">
       <c r="A202" s="7">
         <v>202</v>
       </c>
       <c r="B202" s="8" t="str">
-        <f t="shared" si="4"/>
-        <v>5.30.3.svg</v>
+        <f t="shared" si="5"/>
+        <v>5.32.1.svg</v>
       </c>
       <c r="C202" s="9" t="s">
+        <v>522</v>
+      </c>
+      <c r="D202" s="10" t="s">
         <v>523</v>
       </c>
-      <c r="D202" s="10" t="s">
-        <v>520</v>
-      </c>
       <c r="E202" s="11" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="203" ht="15.75" spans="1:5">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5">
       <c r="A203" s="7">
         <v>203</v>
       </c>
       <c r="B203" s="8" t="str">
-        <f t="shared" si="4"/>
-        <v>5.31.svg</v>
+        <f t="shared" si="5"/>
+        <v>5.32.2.svg</v>
       </c>
       <c r="C203" s="9" t="s">
+        <v>525</v>
+      </c>
+      <c r="D203" s="10" t="s">
+        <v>523</v>
+      </c>
+      <c r="E203" s="11" t="s">
         <v>524</v>
       </c>
-      <c r="D203" s="10" t="s">
-        <v>525</v>
-      </c>
-      <c r="E203" s="11" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="204" ht="15.75" spans="1:5">
+    </row>
+    <row r="204" spans="1:5">
       <c r="A204" s="7">
         <v>204</v>
       </c>
       <c r="B204" s="8" t="str">
-        <f t="shared" si="4"/>
-        <v>5.32.1.svg</v>
+        <f t="shared" si="5"/>
+        <v>5.32.3.svg</v>
       </c>
       <c r="C204" s="9" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="D204" s="10" t="s">
-        <v>528</v>
+        <v>523</v>
       </c>
       <c r="E204" s="11" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="205" ht="15.75" spans="1:5">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="205" ht="31.5" spans="1:5">
       <c r="A205" s="7">
         <v>205</v>
       </c>
       <c r="B205" s="8" t="str">
-        <f t="shared" si="4"/>
-        <v>5.32.2.svg</v>
+        <f t="shared" si="5"/>
+        <v>5.33.svg</v>
       </c>
       <c r="C205" s="9" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="D205" s="10" t="s">
         <v>528</v>
@@ -6869,22 +6848,22 @@
         <v>529</v>
       </c>
     </row>
-    <row r="206" ht="15.75" spans="1:5">
+    <row r="206" ht="31.5" spans="1:5">
       <c r="A206" s="7">
         <v>206</v>
       </c>
       <c r="B206" s="8" t="str">
-        <f t="shared" si="4"/>
-        <v>5.32.3.svg</v>
+        <f t="shared" si="5"/>
+        <v>5.34.1.svg</v>
       </c>
       <c r="C206" s="9" t="s">
+        <v>530</v>
+      </c>
+      <c r="D206" s="10" t="s">
         <v>531</v>
       </c>
-      <c r="D206" s="10" t="s">
-        <v>528</v>
-      </c>
       <c r="E206" s="11" t="s">
-        <v>529</v>
+        <v>532</v>
       </c>
     </row>
     <row r="207" ht="31.5" spans="1:5">
@@ -6892,16 +6871,16 @@
         <v>207</v>
       </c>
       <c r="B207" s="8" t="str">
-        <f t="shared" si="4"/>
-        <v>5.33.svg</v>
+        <f t="shared" si="5"/>
+        <v>5.34.2.svg</v>
       </c>
       <c r="C207" s="9" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="D207" s="10" t="s">
-        <v>533</v>
-      </c>
-      <c r="E207" s="11" t="s">
+        <v>531</v>
+      </c>
+      <c r="E207" s="10" t="s">
         <v>534</v>
       </c>
     </row>
@@ -6910,8 +6889,8 @@
         <v>208</v>
       </c>
       <c r="B208" s="8" t="str">
-        <f t="shared" si="4"/>
-        <v>5.34.1.svg</v>
+        <f t="shared" si="5"/>
+        <v>5.35.svg</v>
       </c>
       <c r="C208" s="9" t="s">
         <v>535</v>
@@ -6923,22 +6902,22 @@
         <v>537</v>
       </c>
     </row>
-    <row r="209" ht="31.5" spans="1:5">
+    <row r="209" spans="1:5">
       <c r="A209" s="7">
         <v>209</v>
       </c>
       <c r="B209" s="8" t="str">
-        <f t="shared" si="4"/>
-        <v>5.34.2.svg</v>
+        <f t="shared" si="5"/>
+        <v>5.36.svg</v>
       </c>
       <c r="C209" s="9" t="s">
         <v>538</v>
       </c>
       <c r="D209" s="10" t="s">
-        <v>536</v>
-      </c>
-      <c r="E209" s="10" t="s">
         <v>539</v>
+      </c>
+      <c r="E209" s="11" t="s">
+        <v>540</v>
       </c>
     </row>
     <row r="210" ht="31.5" spans="1:5">
@@ -6946,62 +6925,60 @@
         <v>210</v>
       </c>
       <c r="B210" s="8" t="str">
-        <f t="shared" si="4"/>
-        <v>5.35.svg</v>
+        <f t="shared" si="5"/>
+        <v>5.37.svg</v>
       </c>
       <c r="C210" s="9" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="D210" s="10" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="E210" s="11" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="211" ht="15.75" spans="1:5">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="211" ht="47.25" spans="1:5">
       <c r="A211" s="7">
         <v>211</v>
       </c>
       <c r="B211" s="8" t="str">
-        <f t="shared" si="4"/>
-        <v>5.36.svg</v>
+        <f t="shared" si="5"/>
+        <v>5.38.svg</v>
       </c>
       <c r="C211" s="9" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="D211" s="10" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="E211" s="11" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="212" ht="31.5" spans="1:5">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5">
       <c r="A212" s="7">
         <v>212</v>
       </c>
       <c r="B212" s="8" t="str">
-        <f t="shared" si="4"/>
-        <v>5.37.svg</v>
+        <f t="shared" si="5"/>
+        <v>5.39.svg</v>
       </c>
       <c r="C212" s="9" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="D212" s="10" t="s">
-        <v>547</v>
-      </c>
-      <c r="E212" s="11" t="s">
         <v>548</v>
       </c>
+      <c r="E212" s="11"/>
     </row>
     <row r="213" ht="47.25" spans="1:5">
       <c r="A213" s="7">
         <v>213</v>
       </c>
       <c r="B213" s="8" t="str">
-        <f t="shared" si="4"/>
-        <v>5.38.svg</v>
+        <f t="shared" si="5"/>
+        <v>5.40.svg</v>
       </c>
       <c r="C213" s="9" t="s">
         <v>549</v>
@@ -7013,13 +6990,13 @@
         <v>551</v>
       </c>
     </row>
-    <row r="214" ht="15.75" spans="1:5">
+    <row r="214" spans="1:5">
       <c r="A214" s="7">
         <v>214</v>
       </c>
       <c r="B214" s="8" t="str">
-        <f t="shared" si="4"/>
-        <v>5.39.svg</v>
+        <f t="shared" si="5"/>
+        <v>5.41.svg</v>
       </c>
       <c r="C214" s="9" t="s">
         <v>552</v>
@@ -7034,8 +7011,8 @@
         <v>215</v>
       </c>
       <c r="B215" s="8" t="str">
-        <f t="shared" si="4"/>
-        <v>5.40.svg</v>
+        <f t="shared" si="5"/>
+        <v>5.42.svg</v>
       </c>
       <c r="C215" s="9" t="s">
         <v>554</v>
@@ -7047,13 +7024,13 @@
         <v>556</v>
       </c>
     </row>
-    <row r="216" ht="15.75" spans="1:5">
+    <row r="216" ht="47.25" spans="1:5">
       <c r="A216" s="7">
         <v>216</v>
       </c>
       <c r="B216" s="8" t="str">
-        <f t="shared" si="4"/>
-        <v>5.41.svg</v>
+        <f t="shared" si="5"/>
+        <v>5.43.svg</v>
       </c>
       <c r="C216" s="9" t="s">
         <v>557</v>
@@ -7061,33 +7038,33 @@
       <c r="D216" s="10" t="s">
         <v>558</v>
       </c>
-      <c r="E216" s="11"/>
-    </row>
-    <row r="217" ht="47.25" spans="1:5">
+      <c r="E216" s="11" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5">
       <c r="A217" s="7">
         <v>217</v>
       </c>
       <c r="B217" s="8" t="str">
-        <f t="shared" si="4"/>
-        <v>5.42.svg</v>
+        <f t="shared" si="5"/>
+        <v>6.1.svg</v>
       </c>
       <c r="C217" s="9" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="D217" s="10" t="s">
-        <v>560</v>
-      </c>
-      <c r="E217" s="11" t="s">
         <v>561</v>
       </c>
-    </row>
-    <row r="218" ht="47.25" spans="1:5">
+      <c r="E217" s="11"/>
+    </row>
+    <row r="218" spans="1:5">
       <c r="A218" s="7">
         <v>218</v>
       </c>
       <c r="B218" s="8" t="str">
-        <f t="shared" si="4"/>
-        <v>5.43.svg</v>
+        <f t="shared" si="5"/>
+        <v>6.2.svg</v>
       </c>
       <c r="C218" s="9" t="s">
         <v>562</v>
@@ -7095,35 +7072,33 @@
       <c r="D218" s="10" t="s">
         <v>563</v>
       </c>
-      <c r="E218" s="11" t="s">
-        <v>564</v>
-      </c>
-    </row>
-    <row r="219" ht="31.5" spans="1:5">
+      <c r="E218" s="11"/>
+    </row>
+    <row r="219" spans="1:5">
       <c r="A219" s="7">
         <v>219</v>
       </c>
       <c r="B219" s="8" t="str">
-        <f t="shared" si="4"/>
-        <v>5.44.svg</v>
+        <f t="shared" si="5"/>
+        <v>6.3.1.svg</v>
       </c>
       <c r="C219" s="9" t="s">
+        <v>564</v>
+      </c>
+      <c r="D219" s="10" t="s">
         <v>565</v>
       </c>
-      <c r="D219" s="10" t="s">
+      <c r="E219" s="11" t="s">
         <v>566</v>
       </c>
-      <c r="E219" s="11" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="220" ht="15.75" spans="1:5">
+    </row>
+    <row r="220" spans="1:5">
       <c r="A220" s="7">
         <v>220</v>
       </c>
       <c r="B220" s="8" t="str">
-        <f t="shared" si="4"/>
-        <v>6.1.svg</v>
+        <f t="shared" si="5"/>
+        <v>6.3.2.svg</v>
       </c>
       <c r="C220" s="9" t="s">
         <v>567</v>
@@ -7133,13 +7108,13 @@
       </c>
       <c r="E220" s="11"/>
     </row>
-    <row r="221" ht="15.75" spans="1:5">
+    <row r="221" spans="1:5">
       <c r="A221" s="7">
         <v>221</v>
       </c>
       <c r="B221" s="8" t="str">
-        <f t="shared" si="4"/>
-        <v>6.2.svg</v>
+        <f t="shared" si="5"/>
+        <v>6.3.3.svg</v>
       </c>
       <c r="C221" s="9" t="s">
         <v>569</v>
@@ -7149,13 +7124,13 @@
       </c>
       <c r="E221" s="11"/>
     </row>
-    <row r="222" ht="15.75" spans="1:5">
+    <row r="222" spans="1:5">
       <c r="A222" s="7">
         <v>222</v>
       </c>
       <c r="B222" s="8" t="str">
-        <f t="shared" si="4"/>
-        <v>6.3.1.svg</v>
+        <f t="shared" si="5"/>
+        <v>6.3.4.svg</v>
       </c>
       <c r="C222" s="9" t="s">
         <v>571</v>
@@ -7164,32 +7139,34 @@
         <v>572</v>
       </c>
       <c r="E222" s="11" t="s">
-        <v>573</v>
-      </c>
-    </row>
-    <row r="223" ht="15.75" spans="1:5">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="223" ht="31.5" spans="1:5">
       <c r="A223" s="7">
         <v>223</v>
       </c>
       <c r="B223" s="8" t="str">
-        <f t="shared" si="4"/>
-        <v>6.3.2.svg</v>
+        <f t="shared" si="5"/>
+        <v>6.3.5.svg</v>
       </c>
       <c r="C223" s="9" t="s">
+        <v>573</v>
+      </c>
+      <c r="D223" s="10" t="s">
         <v>574</v>
       </c>
-      <c r="D223" s="10" t="s">
+      <c r="E223" s="11" t="s">
         <v>575</v>
       </c>
-      <c r="E223" s="11"/>
-    </row>
-    <row r="224" ht="15.75" spans="1:5">
+    </row>
+    <row r="224" spans="1:5">
       <c r="A224" s="7">
         <v>224</v>
       </c>
       <c r="B224" s="8" t="str">
-        <f t="shared" si="4"/>
-        <v>6.3.3.svg</v>
+        <f t="shared" si="5"/>
+        <v>6.3.6.svg</v>
       </c>
       <c r="C224" s="9" t="s">
         <v>576</v>
@@ -7199,13 +7176,13 @@
       </c>
       <c r="E224" s="11"/>
     </row>
-    <row r="225" ht="15.75" spans="1:5">
+    <row r="225" spans="1:5">
       <c r="A225" s="7">
         <v>225</v>
       </c>
       <c r="B225" s="8" t="str">
-        <f t="shared" si="4"/>
-        <v>6.3.4.svg</v>
+        <f t="shared" si="5"/>
+        <v>6.3.7.svg</v>
       </c>
       <c r="C225" s="9" t="s">
         <v>578</v>
@@ -7213,17 +7190,15 @@
       <c r="D225" s="10" t="s">
         <v>579</v>
       </c>
-      <c r="E225" s="11" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="226" ht="31.5" spans="1:5">
+      <c r="E225" s="11"/>
+    </row>
+    <row r="226" spans="1:5">
       <c r="A226" s="7">
         <v>226</v>
       </c>
       <c r="B226" s="8" t="str">
-        <f t="shared" si="4"/>
-        <v>6.3.5.svg</v>
+        <f t="shared" si="5"/>
+        <v>6.4.svg</v>
       </c>
       <c r="C226" s="9" t="s">
         <v>580</v>
@@ -7231,512 +7206,516 @@
       <c r="D226" s="10" t="s">
         <v>581</v>
       </c>
-      <c r="E226" s="11" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="227" ht="15.75" spans="1:5">
+      <c r="E226" s="11"/>
+    </row>
+    <row r="227" spans="1:5">
       <c r="A227" s="7">
         <v>227</v>
       </c>
       <c r="B227" s="8" t="str">
-        <f t="shared" si="4"/>
-        <v>6.3.6.svg</v>
+        <f t="shared" si="5"/>
+        <v>6.5.svg</v>
       </c>
       <c r="C227" s="9" t="s">
+        <v>582</v>
+      </c>
+      <c r="D227" s="10" t="s">
         <v>583</v>
       </c>
-      <c r="D227" s="10" t="s">
-        <v>584</v>
-      </c>
       <c r="E227" s="11"/>
     </row>
-    <row r="228" ht="15.75" spans="1:5">
+    <row r="228" spans="1:5">
       <c r="A228" s="7">
         <v>228</v>
       </c>
       <c r="B228" s="8" t="str">
-        <f t="shared" si="4"/>
-        <v>6.3.7.svg</v>
+        <f t="shared" si="5"/>
+        <v>6.6.svg</v>
       </c>
       <c r="C228" s="9" t="s">
+        <v>584</v>
+      </c>
+      <c r="D228" s="10" t="s">
         <v>585</v>
       </c>
-      <c r="D228" s="10" t="s">
-        <v>586</v>
-      </c>
       <c r="E228" s="11"/>
     </row>
-    <row r="229" ht="15.75" spans="1:5">
+    <row r="229" spans="1:5">
       <c r="A229" s="7">
         <v>229</v>
       </c>
       <c r="B229" s="8" t="str">
-        <f t="shared" si="4"/>
-        <v>6.4.svg</v>
+        <f t="shared" si="5"/>
+        <v>6.7.svg</v>
       </c>
       <c r="C229" s="9" t="s">
+        <v>586</v>
+      </c>
+      <c r="D229" s="10" t="s">
         <v>587</v>
       </c>
-      <c r="D229" s="10" t="s">
-        <v>588</v>
-      </c>
       <c r="E229" s="11"/>
     </row>
-    <row r="230" ht="15.75" spans="1:5">
+    <row r="230" spans="1:5">
       <c r="A230" s="7">
         <v>230</v>
       </c>
       <c r="B230" s="8" t="str">
-        <f t="shared" si="4"/>
-        <v>6.5.svg</v>
+        <f t="shared" ref="B230:B293" si="6">C230&amp;".svg"</f>
+        <v>6.8.svg</v>
       </c>
       <c r="C230" s="9" t="s">
+        <v>588</v>
+      </c>
+      <c r="D230" s="10" t="s">
         <v>589</v>
       </c>
-      <c r="D230" s="10" t="s">
-        <v>590</v>
-      </c>
       <c r="E230" s="11"/>
     </row>
-    <row r="231" ht="15.75" spans="1:5">
+    <row r="231" spans="1:5">
       <c r="A231" s="7">
         <v>231</v>
       </c>
       <c r="B231" s="8" t="str">
-        <f t="shared" si="4"/>
-        <v>6.6.svg</v>
+        <f t="shared" si="6"/>
+        <v>6.9.svg</v>
       </c>
       <c r="C231" s="9" t="s">
+        <v>590</v>
+      </c>
+      <c r="D231" s="10" t="s">
         <v>591</v>
       </c>
-      <c r="D231" s="10" t="s">
-        <v>592</v>
-      </c>
       <c r="E231" s="11"/>
     </row>
-    <row r="232" ht="15.75" spans="1:5">
+    <row r="232" spans="1:5">
       <c r="A232" s="7">
         <v>232</v>
       </c>
       <c r="B232" s="8" t="str">
-        <f t="shared" si="4"/>
-        <v>6.7.svg</v>
+        <f t="shared" si="6"/>
+        <v>6.10.svg</v>
       </c>
       <c r="C232" s="9" t="s">
+        <v>592</v>
+      </c>
+      <c r="D232" s="10" t="s">
         <v>593</v>
       </c>
-      <c r="D232" s="10" t="s">
-        <v>594</v>
-      </c>
       <c r="E232" s="11"/>
     </row>
-    <row r="233" ht="15.75" spans="1:5">
+    <row r="233" spans="1:5">
       <c r="A233" s="7">
         <v>233</v>
       </c>
       <c r="B233" s="8" t="str">
-        <f t="shared" ref="B233:B296" si="5">C233&amp;".svg"</f>
-        <v>6.8.svg</v>
+        <f t="shared" si="6"/>
+        <v>6.11.svg</v>
       </c>
       <c r="C233" s="9" t="s">
+        <v>594</v>
+      </c>
+      <c r="D233" s="10" t="s">
         <v>595</v>
       </c>
-      <c r="D233" s="10" t="s">
-        <v>596</v>
-      </c>
       <c r="E233" s="11"/>
     </row>
-    <row r="234" ht="15.75" spans="1:5">
+    <row r="234" spans="1:5">
       <c r="A234" s="7">
         <v>234</v>
       </c>
       <c r="B234" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>6.9.svg</v>
+        <f t="shared" si="6"/>
+        <v>6.12.1.svg</v>
       </c>
       <c r="C234" s="9" t="s">
+        <v>596</v>
+      </c>
+      <c r="D234" s="10" t="s">
         <v>597</v>
       </c>
-      <c r="D234" s="10" t="s">
-        <v>598</v>
-      </c>
       <c r="E234" s="11"/>
     </row>
-    <row r="235" ht="15.75" spans="1:5">
+    <row r="235" spans="1:5">
       <c r="A235" s="7">
         <v>235</v>
       </c>
       <c r="B235" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>6.10.svg</v>
+        <f t="shared" si="6"/>
+        <v>6.12.2.svg</v>
       </c>
       <c r="C235" s="9" t="s">
+        <v>598</v>
+      </c>
+      <c r="D235" s="10" t="s">
         <v>599</v>
       </c>
-      <c r="D235" s="10" t="s">
-        <v>600</v>
-      </c>
       <c r="E235" s="11"/>
     </row>
-    <row r="236" ht="15.75" spans="1:5">
+    <row r="236" spans="1:5">
       <c r="A236" s="7">
         <v>236</v>
       </c>
       <c r="B236" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>6.11.svg</v>
+        <f t="shared" si="6"/>
+        <v>6.13.svg</v>
       </c>
       <c r="C236" s="9" t="s">
+        <v>600</v>
+      </c>
+      <c r="D236" s="10" t="s">
         <v>601</v>
       </c>
-      <c r="D236" s="10" t="s">
-        <v>602</v>
-      </c>
       <c r="E236" s="11"/>
     </row>
-    <row r="237" ht="15.75" spans="1:5">
+    <row r="237" spans="1:5">
       <c r="A237" s="7">
         <v>237</v>
       </c>
       <c r="B237" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>6.12.1.svg</v>
+        <f t="shared" si="6"/>
+        <v>6.14.svg</v>
       </c>
       <c r="C237" s="9" t="s">
+        <v>602</v>
+      </c>
+      <c r="D237" s="10" t="s">
         <v>603</v>
       </c>
-      <c r="D237" s="10" t="s">
-        <v>604</v>
-      </c>
       <c r="E237" s="11"/>
     </row>
-    <row r="238" ht="15.75" spans="1:5">
+    <row r="238" spans="1:5">
       <c r="A238" s="7">
         <v>238</v>
       </c>
       <c r="B238" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>6.12.2.svg</v>
+        <f t="shared" si="6"/>
+        <v>6.15.svg</v>
       </c>
       <c r="C238" s="9" t="s">
+        <v>604</v>
+      </c>
+      <c r="D238" s="10" t="s">
         <v>605</v>
       </c>
-      <c r="D238" s="10" t="s">
-        <v>606</v>
-      </c>
       <c r="E238" s="11"/>
     </row>
-    <row r="239" ht="15.75" spans="1:5">
+    <row r="239" ht="31.5" spans="1:5">
       <c r="A239" s="7">
         <v>239</v>
       </c>
       <c r="B239" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>6.13.svg</v>
+        <f t="shared" si="6"/>
+        <v>6.16.svg</v>
       </c>
       <c r="C239" s="9" t="s">
+        <v>606</v>
+      </c>
+      <c r="D239" s="10" t="s">
         <v>607</v>
       </c>
-      <c r="D239" s="10" t="s">
-        <v>608</v>
-      </c>
-      <c r="E239" s="11"/>
-    </row>
-    <row r="240" ht="15.75" spans="1:5">
+      <c r="E239" s="11" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="240" ht="47.25" spans="1:5">
       <c r="A240" s="7">
         <v>240</v>
       </c>
       <c r="B240" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>6.14.svg</v>
+        <f t="shared" si="6"/>
+        <v>7.1.1.svg</v>
       </c>
       <c r="C240" s="9" t="s">
+        <v>608</v>
+      </c>
+      <c r="D240" s="10" t="s">
         <v>609</v>
       </c>
-      <c r="D240" s="10" t="s">
+      <c r="E240" s="11" t="s">
         <v>610</v>
       </c>
-      <c r="E240" s="11"/>
-    </row>
-    <row r="241" ht="15.75" spans="1:5">
+    </row>
+    <row r="241" ht="31.5" spans="1:5">
       <c r="A241" s="7">
         <v>241</v>
       </c>
       <c r="B241" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>6.15.svg</v>
+        <f t="shared" si="6"/>
+        <v>7.1.2.svg</v>
       </c>
       <c r="C241" s="9" t="s">
         <v>611</v>
       </c>
       <c r="D241" s="10" t="s">
+        <v>609</v>
+      </c>
+      <c r="E241" s="10" t="s">
         <v>612</v>
       </c>
-      <c r="E241" s="11"/>
-    </row>
-    <row r="242" ht="31.5" spans="1:5">
+    </row>
+    <row r="242" spans="1:5">
       <c r="A242" s="7">
         <v>242</v>
       </c>
       <c r="B242" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>6.16.svg</v>
+        <f t="shared" si="6"/>
+        <v>7.1.3.svg</v>
       </c>
       <c r="C242" s="9" t="s">
         <v>613</v>
       </c>
       <c r="D242" s="10" t="s">
+        <v>609</v>
+      </c>
+      <c r="E242" s="10" t="s">
         <v>614</v>
       </c>
-      <c r="E242" s="11" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="243" ht="47.25" spans="1:5">
+    </row>
+    <row r="243" spans="1:5">
       <c r="A243" s="7">
         <v>243</v>
       </c>
       <c r="B243" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>7.1.1.svg</v>
+        <f t="shared" si="6"/>
+        <v>7.1.4.svg</v>
       </c>
       <c r="C243" s="9" t="s">
         <v>615</v>
       </c>
       <c r="D243" s="10" t="s">
-        <v>616</v>
-      </c>
-      <c r="E243" s="11" t="s">
-        <v>617</v>
-      </c>
-    </row>
-    <row r="244" ht="31.5" spans="1:5">
+        <v>609</v>
+      </c>
+      <c r="E243" s="10" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="244" ht="47.25" spans="1:5">
       <c r="A244" s="7">
         <v>244</v>
       </c>
       <c r="B244" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>7.1.2.svg</v>
+        <f t="shared" si="6"/>
+        <v>7.2.1.svg</v>
       </c>
       <c r="C244" s="9" t="s">
+        <v>616</v>
+      </c>
+      <c r="D244" s="10" t="s">
+        <v>617</v>
+      </c>
+      <c r="E244" s="11" t="s">
         <v>618</v>
       </c>
-      <c r="D244" s="10" t="s">
-        <v>616</v>
-      </c>
-      <c r="E244" s="10" t="s">
-        <v>619</v>
-      </c>
-    </row>
-    <row r="245" ht="15.75" spans="1:5">
+    </row>
+    <row r="245" ht="47.25" spans="1:5">
       <c r="A245" s="7">
         <v>245</v>
       </c>
       <c r="B245" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>7.1.3.svg</v>
+        <f t="shared" si="6"/>
+        <v>7.2.2.svg</v>
       </c>
       <c r="C245" s="9" t="s">
+        <v>619</v>
+      </c>
+      <c r="D245" s="10" t="s">
+        <v>617</v>
+      </c>
+      <c r="E245" s="10" t="s">
         <v>620</v>
       </c>
-      <c r="D245" s="10" t="s">
-        <v>616</v>
-      </c>
-      <c r="E245" s="10" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="246" ht="15.75" spans="1:5">
+    </row>
+    <row r="246" spans="1:5">
       <c r="A246" s="7">
         <v>246</v>
       </c>
       <c r="B246" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>7.1.4.svg</v>
+        <f t="shared" si="6"/>
+        <v>7.2.3.svg</v>
       </c>
       <c r="C246" s="9" t="s">
+        <v>621</v>
+      </c>
+      <c r="D246" s="10" t="s">
+        <v>617</v>
+      </c>
+      <c r="E246" s="10" t="s">
         <v>622</v>
       </c>
-      <c r="D246" s="10" t="s">
-        <v>616</v>
-      </c>
-      <c r="E246" s="10" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="247" ht="47.25" spans="1:5">
+    </row>
+    <row r="247" ht="31.5" spans="1:5">
       <c r="A247" s="7">
         <v>247</v>
       </c>
       <c r="B247" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>7.2.1.svg</v>
+        <f t="shared" si="6"/>
+        <v>7.2.4.svg</v>
       </c>
       <c r="C247" s="9" t="s">
         <v>623</v>
       </c>
       <c r="D247" s="10" t="s">
+        <v>617</v>
+      </c>
+      <c r="E247" s="10" t="s">
         <v>624</v>
       </c>
-      <c r="E247" s="11" t="s">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="248" ht="47.25" spans="1:5">
+    </row>
+    <row r="248" ht="31.5" spans="1:5">
       <c r="A248" s="7">
         <v>248</v>
       </c>
       <c r="B248" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>7.2.2.svg</v>
+        <f t="shared" si="6"/>
+        <v>7.2.5.svg</v>
       </c>
       <c r="C248" s="9" t="s">
+        <v>625</v>
+      </c>
+      <c r="D248" s="10" t="s">
+        <v>617</v>
+      </c>
+      <c r="E248" s="10" t="s">
         <v>626</v>
       </c>
-      <c r="D248" s="10" t="s">
-        <v>624</v>
-      </c>
-      <c r="E248" s="10" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="249" ht="15.75" spans="1:5">
+    </row>
+    <row r="249" ht="31.5" spans="1:5">
       <c r="A249" s="7">
         <v>249</v>
       </c>
       <c r="B249" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>7.2.3.svg</v>
+        <f t="shared" si="6"/>
+        <v>7.2.6.svg</v>
       </c>
       <c r="C249" s="9" t="s">
-        <v>628</v>
-      </c>
-      <c r="D249" s="10" t="s">
-        <v>624</v>
-      </c>
+        <v>627</v>
+      </c>
+      <c r="D249" s="10"/>
       <c r="E249" s="10" t="s">
-        <v>629</v>
-      </c>
-    </row>
-    <row r="250" ht="31.5" spans="1:5">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="250" ht="47.25" spans="1:5">
       <c r="A250" s="7">
         <v>250</v>
       </c>
       <c r="B250" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>7.2.4.svg</v>
+        <f t="shared" si="6"/>
+        <v>7.3.1.svg</v>
       </c>
       <c r="C250" s="9" t="s">
+        <v>628</v>
+      </c>
+      <c r="D250" s="10" t="s">
+        <v>629</v>
+      </c>
+      <c r="E250" s="11" t="s">
         <v>630</v>
       </c>
-      <c r="D250" s="10" t="s">
-        <v>624</v>
-      </c>
-      <c r="E250" s="10" t="s">
-        <v>631</v>
-      </c>
-    </row>
-    <row r="251" ht="31.5" spans="1:5">
+    </row>
+    <row r="251" spans="1:5">
       <c r="A251" s="7">
         <v>251</v>
       </c>
       <c r="B251" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>7.2.5.svg</v>
+        <f t="shared" si="6"/>
+        <v>7.3.2.svg</v>
       </c>
       <c r="C251" s="9" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="D251" s="10" t="s">
-        <v>624</v>
-      </c>
-      <c r="E251" s="10" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="252" ht="31.5" spans="1:5">
+        <v>629</v>
+      </c>
+      <c r="E251" s="11"/>
+    </row>
+    <row r="252" spans="1:5">
       <c r="A252" s="7">
         <v>252</v>
       </c>
       <c r="B252" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>7.2.6.svg</v>
+        <f t="shared" si="6"/>
+        <v>7.3.3.svg</v>
       </c>
       <c r="C252" s="9" t="s">
-        <v>634</v>
-      </c>
-      <c r="D252" s="10"/>
-      <c r="E252" s="10" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="253" ht="47.25" spans="1:5">
+        <v>632</v>
+      </c>
+      <c r="D252" s="10" t="s">
+        <v>629</v>
+      </c>
+      <c r="E252" s="11"/>
+    </row>
+    <row r="253" ht="110.25" spans="1:5">
       <c r="A253" s="7">
         <v>253</v>
       </c>
       <c r="B253" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>7.3.1.svg</v>
+        <f t="shared" si="6"/>
+        <v>7.4.1.svg</v>
       </c>
       <c r="C253" s="9" t="s">
+        <v>633</v>
+      </c>
+      <c r="D253" s="10" t="s">
+        <v>634</v>
+      </c>
+      <c r="E253" s="11" t="s">
         <v>635</v>
       </c>
-      <c r="D253" s="10" t="s">
-        <v>636</v>
-      </c>
-      <c r="E253" s="11" t="s">
-        <v>637</v>
-      </c>
-    </row>
-    <row r="254" ht="15.75" spans="1:5">
+    </row>
+    <row r="254" ht="110.25" spans="1:5">
       <c r="A254" s="7">
         <v>254</v>
       </c>
       <c r="B254" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>7.3.2.svg</v>
+        <f t="shared" si="6"/>
+        <v>7.4.2.svg</v>
       </c>
       <c r="C254" s="9" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="D254" s="10" t="s">
-        <v>636</v>
-      </c>
-      <c r="E254" s="11"/>
-    </row>
-    <row r="255" ht="15.75" spans="1:5">
+        <v>634</v>
+      </c>
+      <c r="E254" s="11" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="255" ht="110.25" spans="1:5">
       <c r="A255" s="7">
         <v>255</v>
       </c>
       <c r="B255" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>7.3.3.svg</v>
+        <f t="shared" si="6"/>
+        <v>7.4.3.svg</v>
       </c>
       <c r="C255" s="9" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="D255" s="10" t="s">
-        <v>636</v>
-      </c>
-      <c r="E255" s="11"/>
+        <v>634</v>
+      </c>
+      <c r="E255" s="11" t="s">
+        <v>635</v>
+      </c>
     </row>
     <row r="256" ht="110.25" spans="1:5">
       <c r="A256" s="7">
         <v>256</v>
       </c>
       <c r="B256" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>7.4.1.svg</v>
+        <f t="shared" si="6"/>
+        <v>7.4.4.svg</v>
       </c>
       <c r="C256" s="9" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="D256" s="10" t="s">
-        <v>641</v>
+        <v>634</v>
       </c>
       <c r="E256" s="11" t="s">
-        <v>642</v>
+        <v>635</v>
       </c>
     </row>
     <row r="257" ht="110.25" spans="1:5">
@@ -7744,17 +7723,17 @@
         <v>257</v>
       </c>
       <c r="B257" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>7.4.2.svg</v>
+        <f t="shared" si="6"/>
+        <v>7.4.5.svg</v>
       </c>
       <c r="C257" s="9" t="s">
-        <v>643</v>
+        <v>639</v>
       </c>
       <c r="D257" s="10" t="s">
-        <v>641</v>
+        <v>634</v>
       </c>
       <c r="E257" s="11" t="s">
-        <v>642</v>
+        <v>635</v>
       </c>
     </row>
     <row r="258" ht="110.25" spans="1:5">
@@ -7762,17 +7741,17 @@
         <v>258</v>
       </c>
       <c r="B258" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>7.4.3.svg</v>
+        <f t="shared" si="6"/>
+        <v>7.4.6.svg</v>
       </c>
       <c r="C258" s="9" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
       <c r="D258" s="10" t="s">
-        <v>641</v>
+        <v>634</v>
       </c>
       <c r="E258" s="11" t="s">
-        <v>642</v>
+        <v>635</v>
       </c>
     </row>
     <row r="259" ht="110.25" spans="1:5">
@@ -7780,17 +7759,17 @@
         <v>259</v>
       </c>
       <c r="B259" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>7.4.4.svg</v>
+        <f t="shared" si="6"/>
+        <v>7.4.7.svg</v>
       </c>
       <c r="C259" s="9" t="s">
-        <v>645</v>
+        <v>641</v>
       </c>
       <c r="D259" s="10" t="s">
-        <v>641</v>
+        <v>634</v>
       </c>
       <c r="E259" s="11" t="s">
-        <v>642</v>
+        <v>635</v>
       </c>
     </row>
     <row r="260" ht="110.25" spans="1:5">
@@ -7798,98 +7777,94 @@
         <v>260</v>
       </c>
       <c r="B260" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>7.4.5.svg</v>
+        <f t="shared" si="6"/>
+        <v>7.4.8.svg</v>
       </c>
       <c r="C260" s="9" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="D260" s="10" t="s">
-        <v>641</v>
+        <v>634</v>
       </c>
       <c r="E260" s="11" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="261" ht="110.25" spans="1:5">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="261" ht="31.5" spans="1:5">
       <c r="A261" s="7">
         <v>261</v>
       </c>
       <c r="B261" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>7.4.6.svg</v>
+        <f t="shared" si="6"/>
+        <v>7.4.9.svg</v>
       </c>
       <c r="C261" s="9" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
       <c r="D261" s="10" t="s">
-        <v>641</v>
+        <v>644</v>
       </c>
       <c r="E261" s="11" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="262" ht="110.25" spans="1:5">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="262" spans="1:5">
       <c r="A262" s="7">
         <v>262</v>
       </c>
       <c r="B262" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>7.4.7.svg</v>
+        <f t="shared" si="6"/>
+        <v>7.5.1.svg</v>
       </c>
       <c r="C262" s="9" t="s">
+        <v>646</v>
+      </c>
+      <c r="D262" s="10" t="s">
+        <v>647</v>
+      </c>
+      <c r="E262" s="11" t="s">
         <v>648</v>
       </c>
-      <c r="D262" s="10" t="s">
-        <v>641</v>
-      </c>
-      <c r="E262" s="11" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="263" ht="110.25" spans="1:5">
+    </row>
+    <row r="263" spans="1:5">
       <c r="A263" s="7">
         <v>263</v>
       </c>
       <c r="B263" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>7.4.8.svg</v>
+        <f t="shared" si="6"/>
+        <v>7.5.2.svg</v>
       </c>
       <c r="C263" s="9" t="s">
         <v>649</v>
       </c>
       <c r="D263" s="10" t="s">
-        <v>641</v>
-      </c>
-      <c r="E263" s="11" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="264" ht="31.5" spans="1:5">
+        <v>650</v>
+      </c>
+      <c r="E263" s="11"/>
+    </row>
+    <row r="264" spans="1:5">
       <c r="A264" s="7">
         <v>264</v>
       </c>
       <c r="B264" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>7.4.9.svg</v>
+        <f t="shared" si="6"/>
+        <v>7.5.3.svg</v>
       </c>
       <c r="C264" s="9" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="D264" s="10" t="s">
-        <v>651</v>
-      </c>
-      <c r="E264" s="11" t="s">
         <v>652</v>
       </c>
-    </row>
-    <row r="265" ht="15.75" spans="1:5">
+      <c r="E264" s="11"/>
+    </row>
+    <row r="265" spans="1:5">
       <c r="A265" s="7">
         <v>265</v>
       </c>
       <c r="B265" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>7.5.1.svg</v>
+        <f t="shared" si="6"/>
+        <v>7.5.4.svg</v>
       </c>
       <c r="C265" s="9" t="s">
         <v>653</v>
@@ -7901,84 +7876,88 @@
         <v>655</v>
       </c>
     </row>
-    <row r="266" ht="15.75" spans="1:5">
+    <row r="266" spans="1:5">
       <c r="A266" s="7">
         <v>266</v>
       </c>
       <c r="B266" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>7.5.2.svg</v>
+        <f t="shared" si="6"/>
+        <v>7.5.5.svg</v>
       </c>
       <c r="C266" s="9" t="s">
         <v>656</v>
       </c>
       <c r="D266" s="10" t="s">
+        <v>654</v>
+      </c>
+      <c r="E266" s="10" t="s">
         <v>657</v>
       </c>
-      <c r="E266" s="11"/>
-    </row>
-    <row r="267" ht="15.75" spans="1:5">
+    </row>
+    <row r="267" spans="1:5">
       <c r="A267" s="7">
         <v>267</v>
       </c>
       <c r="B267" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>7.5.3.svg</v>
+        <f t="shared" si="6"/>
+        <v>7.5.6.svg</v>
       </c>
       <c r="C267" s="9" t="s">
         <v>658</v>
       </c>
       <c r="D267" s="10" t="s">
-        <v>659</v>
-      </c>
-      <c r="E267" s="11"/>
-    </row>
-    <row r="268" ht="15.75" spans="1:5">
+        <v>654</v>
+      </c>
+      <c r="E267" s="10" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="268" spans="1:5">
       <c r="A268" s="7">
         <v>268</v>
       </c>
       <c r="B268" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>7.5.4.svg</v>
+        <f t="shared" si="6"/>
+        <v>7.5.7.svg</v>
       </c>
       <c r="C268" s="9" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="D268" s="10" t="s">
-        <v>661</v>
-      </c>
-      <c r="E268" s="11" t="s">
-        <v>662</v>
-      </c>
-    </row>
-    <row r="269" ht="15.75" spans="1:5">
+        <v>654</v>
+      </c>
+      <c r="E268" s="10" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="269" ht="31.5" spans="1:5">
       <c r="A269" s="7">
         <v>269</v>
       </c>
       <c r="B269" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>7.5.5.svg</v>
+        <f t="shared" si="6"/>
+        <v>7.6.1 (7.6.10).svg</v>
       </c>
       <c r="C269" s="9" t="s">
-        <v>663</v>
+        <v>660</v>
       </c>
       <c r="D269" s="10" t="s">
         <v>661</v>
       </c>
-      <c r="E269" s="10" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="270" ht="15.75" spans="1:5">
+      <c r="E269" s="11" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="270" ht="47.25" spans="1:5">
       <c r="A270" s="7">
         <v>270</v>
       </c>
       <c r="B270" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>7.5.6.svg</v>
+        <f t="shared" si="6"/>
+        <v>7.6.2 (7.6.11).svg</v>
       </c>
       <c r="C270" s="9" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="D270" s="10" t="s">
         <v>661</v>
@@ -7987,16 +7966,16 @@
         <v>664</v>
       </c>
     </row>
-    <row r="271" ht="15.75" spans="1:5">
+    <row r="271" ht="47.25" spans="1:5">
       <c r="A271" s="7">
         <v>271</v>
       </c>
       <c r="B271" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>7.5.7.svg</v>
+        <f t="shared" si="6"/>
+        <v>7.6.3 (7.6.12).svg</v>
       </c>
       <c r="C271" s="9" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="D271" s="10" t="s">
         <v>661</v>
@@ -8005,22 +7984,22 @@
         <v>664</v>
       </c>
     </row>
-    <row r="272" ht="31.5" spans="1:5">
+    <row r="272" ht="47.25" spans="1:5">
       <c r="A272" s="7">
         <v>272</v>
       </c>
       <c r="B272" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>7.6.1 (7.6.10).svg</v>
+        <f t="shared" si="6"/>
+        <v>7.6.4 (7.6.13).svg</v>
       </c>
       <c r="C272" s="9" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="D272" s="10" t="s">
-        <v>668</v>
-      </c>
-      <c r="E272" s="11" t="s">
-        <v>669</v>
+        <v>661</v>
+      </c>
+      <c r="E272" s="10" t="s">
+        <v>664</v>
       </c>
     </row>
     <row r="273" ht="47.25" spans="1:5">
@@ -8028,17 +8007,17 @@
         <v>273</v>
       </c>
       <c r="B273" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>7.6.2 (7.6.11).svg</v>
+        <f t="shared" si="6"/>
+        <v>7.6.5 (7.6.14).svg</v>
       </c>
       <c r="C273" s="9" t="s">
-        <v>670</v>
+        <v>667</v>
       </c>
       <c r="D273" s="10" t="s">
-        <v>668</v>
+        <v>661</v>
       </c>
       <c r="E273" s="10" t="s">
-        <v>671</v>
+        <v>664</v>
       </c>
     </row>
     <row r="274" ht="47.25" spans="1:5">
@@ -8046,17 +8025,17 @@
         <v>274</v>
       </c>
       <c r="B274" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>7.6.3 (7.6.12).svg</v>
+        <f t="shared" si="6"/>
+        <v>7.6.6 (7.6.15).svg</v>
       </c>
       <c r="C274" s="9" t="s">
-        <v>672</v>
+        <v>668</v>
       </c>
       <c r="D274" s="10" t="s">
-        <v>668</v>
+        <v>661</v>
       </c>
       <c r="E274" s="10" t="s">
-        <v>671</v>
+        <v>664</v>
       </c>
     </row>
     <row r="275" ht="47.25" spans="1:5">
@@ -8064,17 +8043,17 @@
         <v>275</v>
       </c>
       <c r="B275" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>7.6.4 (7.6.13).svg</v>
+        <f t="shared" si="6"/>
+        <v>7.6.7 (7.6.16).svg</v>
       </c>
       <c r="C275" s="9" t="s">
-        <v>673</v>
+        <v>669</v>
       </c>
       <c r="D275" s="10" t="s">
-        <v>668</v>
+        <v>661</v>
       </c>
       <c r="E275" s="10" t="s">
-        <v>671</v>
+        <v>664</v>
       </c>
     </row>
     <row r="276" ht="47.25" spans="1:5">
@@ -8082,17 +8061,17 @@
         <v>276</v>
       </c>
       <c r="B276" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>7.6.5 (7.6.14).svg</v>
+        <f t="shared" si="6"/>
+        <v>7.6.8 (7.6.17).svg</v>
       </c>
       <c r="C276" s="9" t="s">
-        <v>674</v>
+        <v>670</v>
       </c>
       <c r="D276" s="10" t="s">
-        <v>668</v>
+        <v>661</v>
       </c>
       <c r="E276" s="10" t="s">
-        <v>671</v>
+        <v>664</v>
       </c>
     </row>
     <row r="277" ht="47.25" spans="1:5">
@@ -8100,71 +8079,71 @@
         <v>277</v>
       </c>
       <c r="B277" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>7.6.6 (7.6.15).svg</v>
+        <f t="shared" si="6"/>
+        <v>7.6.9 (7.6.18).svg</v>
       </c>
       <c r="C277" s="9" t="s">
-        <v>675</v>
+        <v>671</v>
       </c>
       <c r="D277" s="10" t="s">
-        <v>668</v>
+        <v>661</v>
       </c>
       <c r="E277" s="10" t="s">
-        <v>671</v>
-      </c>
-    </row>
-    <row r="278" ht="47.25" spans="1:5">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="278" ht="31.5" spans="1:5">
       <c r="A278" s="7">
         <v>278</v>
       </c>
       <c r="B278" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>7.6.7 (7.6.16).svg</v>
+        <f t="shared" si="6"/>
+        <v>7.7.svg</v>
       </c>
       <c r="C278" s="9" t="s">
-        <v>676</v>
+        <v>672</v>
       </c>
       <c r="D278" s="10" t="s">
-        <v>668</v>
-      </c>
-      <c r="E278" s="10" t="s">
-        <v>671</v>
-      </c>
-    </row>
-    <row r="279" ht="47.25" spans="1:5">
+        <v>673</v>
+      </c>
+      <c r="E278" s="11" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="279" spans="1:5">
       <c r="A279" s="7">
         <v>279</v>
       </c>
       <c r="B279" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>7.6.8 (7.6.17).svg</v>
+        <f t="shared" si="6"/>
+        <v>7.8.svg</v>
       </c>
       <c r="C279" s="9" t="s">
+        <v>675</v>
+      </c>
+      <c r="D279" s="10" t="s">
+        <v>676</v>
+      </c>
+      <c r="E279" s="11" t="s">
         <v>677</v>
       </c>
-      <c r="D279" s="10" t="s">
-        <v>668</v>
-      </c>
-      <c r="E279" s="10" t="s">
-        <v>671</v>
-      </c>
-    </row>
-    <row r="280" ht="47.25" spans="1:5">
+    </row>
+    <row r="280" ht="31.5" spans="1:5">
       <c r="A280" s="7">
         <v>280</v>
       </c>
       <c r="B280" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>7.6.9 (7.6.18).svg</v>
+        <f t="shared" si="6"/>
+        <v>7.9.svg</v>
       </c>
       <c r="C280" s="9" t="s">
         <v>678</v>
       </c>
       <c r="D280" s="10" t="s">
-        <v>668</v>
-      </c>
-      <c r="E280" s="10" t="s">
-        <v>671</v>
+        <v>679</v>
+      </c>
+      <c r="E280" s="11" t="s">
+        <v>680</v>
       </c>
     </row>
     <row r="281" ht="31.5" spans="1:5">
@@ -8172,35 +8151,35 @@
         <v>281</v>
       </c>
       <c r="B281" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>7.7.svg</v>
+        <f t="shared" si="6"/>
+        <v>7.10.svg</v>
       </c>
       <c r="C281" s="9" t="s">
-        <v>679</v>
+        <v>681</v>
       </c>
       <c r="D281" s="10" t="s">
-        <v>680</v>
+        <v>682</v>
       </c>
       <c r="E281" s="11" t="s">
-        <v>681</v>
-      </c>
-    </row>
-    <row r="282" ht="15.75" spans="1:5">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="282" ht="31.5" spans="1:5">
       <c r="A282" s="7">
         <v>282</v>
       </c>
       <c r="B282" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>7.8.svg</v>
+        <f t="shared" si="6"/>
+        <v>7.11.svg</v>
       </c>
       <c r="C282" s="9" t="s">
-        <v>682</v>
+        <v>684</v>
       </c>
       <c r="D282" s="10" t="s">
-        <v>683</v>
+        <v>685</v>
       </c>
       <c r="E282" s="11" t="s">
-        <v>684</v>
+        <v>686</v>
       </c>
     </row>
     <row r="283" ht="31.5" spans="1:5">
@@ -8208,17 +8187,17 @@
         <v>283</v>
       </c>
       <c r="B283" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>7.9.svg</v>
+        <f t="shared" si="6"/>
+        <v>7.12.svg</v>
       </c>
       <c r="C283" s="9" t="s">
-        <v>685</v>
+        <v>687</v>
       </c>
       <c r="D283" s="10" t="s">
-        <v>686</v>
+        <v>688</v>
       </c>
       <c r="E283" s="11" t="s">
-        <v>687</v>
+        <v>689</v>
       </c>
     </row>
     <row r="284" ht="31.5" spans="1:5">
@@ -8226,17 +8205,17 @@
         <v>284</v>
       </c>
       <c r="B284" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>7.10.svg</v>
+        <f t="shared" si="6"/>
+        <v>7.13.svg</v>
       </c>
       <c r="C284" s="9" t="s">
-        <v>688</v>
+        <v>690</v>
       </c>
       <c r="D284" s="10" t="s">
-        <v>689</v>
+        <v>691</v>
       </c>
       <c r="E284" s="11" t="s">
-        <v>690</v>
+        <v>692</v>
       </c>
     </row>
     <row r="285" ht="31.5" spans="1:5">
@@ -8244,17 +8223,17 @@
         <v>285</v>
       </c>
       <c r="B285" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>7.11.svg</v>
+        <f t="shared" si="6"/>
+        <v>7.14.svg</v>
       </c>
       <c r="C285" s="9" t="s">
-        <v>691</v>
+        <v>693</v>
       </c>
       <c r="D285" s="10" t="s">
-        <v>692</v>
+        <v>694</v>
       </c>
       <c r="E285" s="11" t="s">
-        <v>693</v>
+        <v>695</v>
       </c>
     </row>
     <row r="286" ht="31.5" spans="1:5">
@@ -8262,17 +8241,17 @@
         <v>286</v>
       </c>
       <c r="B286" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>7.12.svg</v>
+        <f t="shared" si="6"/>
+        <v>7.15.svg</v>
       </c>
       <c r="C286" s="9" t="s">
-        <v>694</v>
+        <v>696</v>
       </c>
       <c r="D286" s="10" t="s">
-        <v>695</v>
+        <v>697</v>
       </c>
       <c r="E286" s="11" t="s">
-        <v>696</v>
+        <v>698</v>
       </c>
     </row>
     <row r="287" ht="31.5" spans="1:5">
@@ -8280,35 +8259,35 @@
         <v>287</v>
       </c>
       <c r="B287" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>7.13.svg</v>
+        <f t="shared" si="6"/>
+        <v>7.16.svg</v>
       </c>
       <c r="C287" s="9" t="s">
-        <v>697</v>
+        <v>699</v>
       </c>
       <c r="D287" s="10" t="s">
-        <v>698</v>
+        <v>700</v>
       </c>
       <c r="E287" s="11" t="s">
-        <v>699</v>
-      </c>
-    </row>
-    <row r="288" ht="31.5" spans="1:5">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="288" ht="47.25" spans="1:5">
       <c r="A288" s="7">
         <v>288</v>
       </c>
       <c r="B288" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>7.14.svg</v>
+        <f t="shared" si="6"/>
+        <v>7.17.svg</v>
       </c>
       <c r="C288" s="9" t="s">
-        <v>700</v>
+        <v>702</v>
       </c>
       <c r="D288" s="10" t="s">
-        <v>701</v>
+        <v>703</v>
       </c>
       <c r="E288" s="11" t="s">
-        <v>702</v>
+        <v>704</v>
       </c>
     </row>
     <row r="289" ht="31.5" spans="1:5">
@@ -8316,53 +8295,53 @@
         <v>289</v>
       </c>
       <c r="B289" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>7.15.svg</v>
+        <f t="shared" si="6"/>
+        <v>7.18.svg</v>
       </c>
       <c r="C289" s="9" t="s">
-        <v>703</v>
+        <v>705</v>
       </c>
       <c r="D289" s="10" t="s">
-        <v>704</v>
+        <v>706</v>
       </c>
       <c r="E289" s="11" t="s">
-        <v>705</v>
-      </c>
-    </row>
-    <row r="290" ht="31.5" spans="1:5">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="290" ht="47.25" spans="1:5">
       <c r="A290" s="7">
         <v>290</v>
       </c>
       <c r="B290" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>7.16.svg</v>
+        <f t="shared" si="6"/>
+        <v>7.19.svg</v>
       </c>
       <c r="C290" s="9" t="s">
-        <v>706</v>
+        <v>708</v>
       </c>
       <c r="D290" s="10" t="s">
-        <v>707</v>
+        <v>709</v>
       </c>
       <c r="E290" s="11" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="291" ht="47.25" spans="1:5">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="291" ht="63" spans="1:5">
       <c r="A291" s="7">
         <v>291</v>
       </c>
       <c r="B291" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>7.17.svg</v>
+        <f t="shared" si="6"/>
+        <v>7.20.svg</v>
       </c>
       <c r="C291" s="9" t="s">
-        <v>709</v>
+        <v>711</v>
       </c>
       <c r="D291" s="10" t="s">
-        <v>710</v>
+        <v>712</v>
       </c>
       <c r="E291" s="11" t="s">
-        <v>711</v>
+        <v>713</v>
       </c>
     </row>
     <row r="292" ht="31.5" spans="1:5">
@@ -8370,53 +8349,53 @@
         <v>292</v>
       </c>
       <c r="B292" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>7.18.svg</v>
+        <f t="shared" si="6"/>
+        <v>7.21.svg</v>
       </c>
       <c r="C292" s="9" t="s">
-        <v>712</v>
+        <v>714</v>
       </c>
       <c r="D292" s="10" t="s">
-        <v>713</v>
+        <v>715</v>
       </c>
       <c r="E292" s="11" t="s">
-        <v>714</v>
-      </c>
-    </row>
-    <row r="293" ht="47.25" spans="1:5">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="293" ht="31.5" spans="1:5">
       <c r="A293" s="7">
         <v>293</v>
       </c>
       <c r="B293" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>7.19.svg</v>
+        <f t="shared" si="6"/>
+        <v>7.22.1.svg</v>
       </c>
       <c r="C293" s="9" t="s">
-        <v>715</v>
+        <v>717</v>
       </c>
       <c r="D293" s="10" t="s">
-        <v>716</v>
+        <v>718</v>
       </c>
       <c r="E293" s="11" t="s">
-        <v>717</v>
-      </c>
-    </row>
-    <row r="294" ht="63" spans="1:5">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="294" ht="31.5" spans="1:5">
       <c r="A294" s="7">
         <v>294</v>
       </c>
       <c r="B294" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>7.20.svg</v>
+        <f t="shared" ref="B294:B299" si="7">C294&amp;".svg"</f>
+        <v>7.22.2.svg</v>
       </c>
       <c r="C294" s="9" t="s">
+        <v>720</v>
+      </c>
+      <c r="D294" s="10" t="s">
         <v>718</v>
       </c>
-      <c r="D294" s="10" t="s">
+      <c r="E294" s="11" t="s">
         <v>719</v>
-      </c>
-      <c r="E294" s="11" t="s">
-        <v>720</v>
       </c>
     </row>
     <row r="295" ht="31.5" spans="1:5">
@@ -8424,17 +8403,17 @@
         <v>295</v>
       </c>
       <c r="B295" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>7.21.svg</v>
+        <f t="shared" si="7"/>
+        <v>7.22.3.svg</v>
       </c>
       <c r="C295" s="9" t="s">
         <v>721</v>
       </c>
       <c r="D295" s="10" t="s">
-        <v>722</v>
+        <v>718</v>
       </c>
       <c r="E295" s="11" t="s">
-        <v>723</v>
+        <v>719</v>
       </c>
     </row>
     <row r="296" ht="31.5" spans="1:5">
@@ -8442,124 +8421,70 @@
         <v>296</v>
       </c>
       <c r="B296" s="8" t="str">
-        <f t="shared" si="5"/>
-        <v>7.22.1.svg</v>
+        <f t="shared" si="7"/>
+        <v>7.22.4.svg</v>
       </c>
       <c r="C296" s="9" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="D296" s="10" t="s">
-        <v>725</v>
+        <v>718</v>
       </c>
       <c r="E296" s="11" t="s">
-        <v>726</v>
-      </c>
-    </row>
-    <row r="297" ht="31.5" spans="1:5">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="297" spans="1:5">
       <c r="A297" s="7">
         <v>297</v>
       </c>
       <c r="B297" s="8" t="str">
-        <f t="shared" ref="B297:B302" si="6">C297&amp;".svg"</f>
-        <v>7.22.2.svg</v>
+        <f t="shared" si="7"/>
+        <v>7.23.svg</v>
       </c>
       <c r="C297" s="9" t="s">
-        <v>727</v>
+        <v>723</v>
       </c>
       <c r="D297" s="10" t="s">
+        <v>724</v>
+      </c>
+      <c r="E297" s="11" t="s">
         <v>725</v>
       </c>
-      <c r="E297" s="11" t="s">
-        <v>726</v>
-      </c>
-    </row>
-    <row r="298" ht="31.5" spans="1:5">
+    </row>
+    <row r="298" ht="47.25" spans="1:5">
       <c r="A298" s="7">
         <v>298</v>
       </c>
       <c r="B298" s="8" t="str">
-        <f t="shared" si="6"/>
-        <v>7.22.3.svg</v>
+        <f t="shared" si="7"/>
+        <v>7.24.svg</v>
       </c>
       <c r="C298" s="9" t="s">
+        <v>726</v>
+      </c>
+      <c r="D298" s="10" t="s">
+        <v>727</v>
+      </c>
+      <c r="E298" s="11" t="s">
         <v>728</v>
       </c>
-      <c r="D298" s="10" t="s">
-        <v>725</v>
-      </c>
-      <c r="E298" s="11" t="s">
-        <v>726</v>
-      </c>
-    </row>
-    <row r="299" ht="31.5" spans="1:5">
+    </row>
+    <row r="299" spans="1:5">
       <c r="A299" s="7">
         <v>299</v>
       </c>
       <c r="B299" s="8" t="str">
-        <f t="shared" si="6"/>
-        <v>7.22.4.svg</v>
+        <f t="shared" si="7"/>
+        <v>7.25.svg</v>
       </c>
       <c r="C299" s="9" t="s">
         <v>729</v>
       </c>
       <c r="D299" s="10" t="s">
-        <v>725</v>
+        <v>730</v>
       </c>
       <c r="E299" s="11" t="s">
-        <v>726</v>
-      </c>
-    </row>
-    <row r="300" ht="15.75" spans="1:5">
-      <c r="A300" s="7">
-        <v>300</v>
-      </c>
-      <c r="B300" s="8" t="str">
-        <f t="shared" si="6"/>
-        <v>7.23.svg</v>
-      </c>
-      <c r="C300" s="9" t="s">
-        <v>730</v>
-      </c>
-      <c r="D300" s="10" t="s">
-        <v>731</v>
-      </c>
-      <c r="E300" s="11" t="s">
-        <v>732</v>
-      </c>
-    </row>
-    <row r="301" ht="47.25" spans="1:5">
-      <c r="A301" s="7">
-        <v>301</v>
-      </c>
-      <c r="B301" s="8" t="str">
-        <f t="shared" si="6"/>
-        <v>7.24.svg</v>
-      </c>
-      <c r="C301" s="9" t="s">
-        <v>733</v>
-      </c>
-      <c r="D301" s="10" t="s">
-        <v>734</v>
-      </c>
-      <c r="E301" s="11" t="s">
-        <v>735</v>
-      </c>
-    </row>
-    <row r="302" ht="15.75" spans="1:5">
-      <c r="A302" s="7">
-        <v>302</v>
-      </c>
-      <c r="B302" s="8" t="str">
-        <f t="shared" si="6"/>
-        <v>7.25.svg</v>
-      </c>
-      <c r="C302" s="9" t="s">
-        <v>736</v>
-      </c>
-      <c r="D302" s="10" t="s">
-        <v>737</v>
-      </c>
-      <c r="E302" s="11" t="s">
         <v>326</v>
       </c>
     </row>

</xml_diff>